<commit_message>
changed metrics2 to csv to import
</commit_message>
<xml_diff>
--- a/data/bsa - metrics data2.xlsx
+++ b/data/bsa - metrics data2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59ae7835bc9d2c4d/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slash\Documents\bsa-research\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="518" documentId="8_{29F8CB44-6385-4367-90BC-530F15327FFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1D71A5D0-D7E2-427E-8424-1B0D7F80C5EA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E503966-223A-4F6B-A213-45E7F6F661D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="9" xr2:uid="{011EEE82-27A8-4D35-ACB3-E0118E4D60F0}"/>
   </bookViews>

</xml_diff>